<commit_message>
SaiReddy:hlookup and documentadd for v and h lookup
</commit_message>
<xml_diff>
--- a/Day-12-(Excel).xlsx
+++ b/Day-12-(Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataAnalytics\Excel\Day-12-(Excel)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBAD64A7-F839-453A-BAA4-C10EAB8290E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423620E2-7E2D-4499-8964-EF5CAA58F7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -929,7 +929,7 @@
   <dimension ref="D6:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="E10" sqref="E10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -968,12 +968,30 @@
       <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="E7" s="5" t="str">
+        <f>HLOOKUP(E6,$D$15:$J$17,2,FALSE)</f>
+        <v>automotive sq, near tp road , 400001</v>
+      </c>
+      <c r="F7" s="5" t="str">
+        <f t="shared" ref="F7:J7" si="0">HLOOKUP(F6,$D$15:$J$17,2,FALSE)</f>
+        <v>offline</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D8" s="5" t="s">
@@ -1025,12 +1043,30 @@
       <c r="D10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="E10" s="5" t="str">
+        <f>HLOOKUP(E6,$D$15:$J$17,3,FALSE)</f>
+        <v>nandanvan</v>
+      </c>
+      <c r="F10" s="5" t="str">
+        <f t="shared" ref="F10:J10" si="1">HLOOKUP(F6,$D$15:$J$17,3,FALSE)</f>
+        <v>online</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="1"/>
+        <v>200000</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
     </row>
     <row r="11" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D11" s="5" t="s">

</xml_diff>

<commit_message>
SaiReddy: 5 Examples added of V nad H LOOKUP
</commit_message>
<xml_diff>
--- a/Day-12-(Excel).xlsx
+++ b/Day-12-(Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataAnalytics\Excel\Day-12-(Excel)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423620E2-7E2D-4499-8964-EF5CAA58F7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E051C5F1-D32B-40EB-8EDD-43CA38F3D855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="200">
   <si>
     <t>ARC</t>
   </si>
@@ -177,13 +177,589 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>5 Examples Of Hlookup</t>
+  </si>
+  <si>
+    <t>5 Examples Of Vlookup</t>
+  </si>
+  <si>
+    <t>EMP ID</t>
+  </si>
+  <si>
+    <t>Salesman</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Target Status (IF)</t>
+  </si>
+  <si>
+    <t>Incentive (IF)</t>
+  </si>
+  <si>
+    <t>EMP001</t>
+  </si>
+  <si>
+    <t>Employee_1</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>EMP002</t>
+  </si>
+  <si>
+    <t>Employee_2</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>EMP003</t>
+  </si>
+  <si>
+    <t>Employee_3</t>
+  </si>
+  <si>
+    <t>EMP004</t>
+  </si>
+  <si>
+    <t>Employee_4</t>
+  </si>
+  <si>
+    <t>EMP005</t>
+  </si>
+  <si>
+    <t>Employee_5</t>
+  </si>
+  <si>
+    <t>EMP006</t>
+  </si>
+  <si>
+    <t>Employee_6</t>
+  </si>
+  <si>
+    <t>EMP007</t>
+  </si>
+  <si>
+    <t>Employee_7</t>
+  </si>
+  <si>
+    <t>EMP008</t>
+  </si>
+  <si>
+    <t>Employee_8</t>
+  </si>
+  <si>
+    <t>EMP009</t>
+  </si>
+  <si>
+    <t>Employee_9</t>
+  </si>
+  <si>
+    <t>EMP010</t>
+  </si>
+  <si>
+    <t>Employee_10</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>incomplete</t>
+  </si>
+  <si>
+    <t>Example 1</t>
+  </si>
+  <si>
+    <t>Emp ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>E001</t>
+  </si>
+  <si>
+    <t>Riya Shah</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>E002</t>
+  </si>
+  <si>
+    <t>Arjun Mehta</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>E003</t>
+  </si>
+  <si>
+    <t>Sneha Roy</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>E004</t>
+  </si>
+  <si>
+    <t>Kunal Das</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>S101</t>
+  </si>
+  <si>
+    <t>Meera Singh</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S102</t>
+  </si>
+  <si>
+    <t>Rahul Verma</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>S103</t>
+  </si>
+  <si>
+    <t>Tanya Gupta</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>S104</t>
+  </si>
+  <si>
+    <t>Dev Mishra</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>Flight No</t>
+  </si>
+  <si>
+    <t>Airline</t>
+  </si>
+  <si>
+    <t>Departure</t>
+  </si>
+  <si>
+    <t>Arrival</t>
+  </si>
+  <si>
+    <t>AI202</t>
+  </si>
+  <si>
+    <t>Air India</t>
+  </si>
+  <si>
+    <t>Dubai</t>
+  </si>
+  <si>
+    <t>EK501</t>
+  </si>
+  <si>
+    <t>Emirates</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>BA134</t>
+  </si>
+  <si>
+    <t>British Air</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>LH760</t>
+  </si>
+  <si>
+    <t>Lufthansa</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Reg No</t>
+  </si>
+  <si>
+    <t>Owner Name</t>
+  </si>
+  <si>
+    <t>Vehicle Type</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>MH12AB1234</t>
+  </si>
+  <si>
+    <t>Nikhil Joshi</t>
+  </si>
+  <si>
+    <t>Sedan</t>
+  </si>
+  <si>
+    <t>DL8CAF4321</t>
+  </si>
+  <si>
+    <t>Priya Malhotra</t>
+  </si>
+  <si>
+    <t>SUV</t>
+  </si>
+  <si>
+    <t>KA03MN8765</t>
+  </si>
+  <si>
+    <t>Ravi Kumar</t>
+  </si>
+  <si>
+    <t>Hatchback</t>
+  </si>
+  <si>
+    <t>TN22XY9988</t>
+  </si>
+  <si>
+    <t>Sneha Iyer</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Rent (₹)</t>
+  </si>
+  <si>
+    <t>Groceries (₹)</t>
+  </si>
+  <si>
+    <t>Travel (₹)</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Model A</t>
+  </si>
+  <si>
+    <t>Model B</t>
+  </si>
+  <si>
+    <t>Model C</t>
+  </si>
+  <si>
+    <t>Model D</t>
+  </si>
+  <si>
+    <t>Price (₹)</t>
+  </si>
+  <si>
+    <t>Battery (hrs)</t>
+  </si>
+  <si>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Festival</t>
+  </si>
+  <si>
+    <t>Makar Sankranti</t>
+  </si>
+  <si>
+    <t>✔</t>
+  </si>
+  <si>
+    <t>Holi</t>
+  </si>
+  <si>
+    <t>Eid</t>
+  </si>
+  <si>
+    <t>Buddha Purnima</t>
+  </si>
+  <si>
+    <t>Example 2</t>
+  </si>
+  <si>
+    <t>Example 3</t>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Find course and grade by Student ID.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Lookup Employee Location &amp; Name by Emp ID.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Lookup airline and Arrival by Flight No.</t>
+    </r>
+  </si>
+  <si>
+    <t>Example 4</t>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Lookup vehicle info by registration number.</t>
+    </r>
+  </si>
+  <si>
+    <t>Example 5</t>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Find Department &amp; Sales by Em ID.</t>
+    </r>
+  </si>
+  <si>
+    <t>Vlookup</t>
+  </si>
+  <si>
+    <t>Hlookup</t>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Lookup expenses by month.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Compare features across models.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Lookup scores by student name.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Use</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Lookup festivals by month.</t>
+    </r>
+  </si>
+  <si>
+    <t>Salesman Name</t>
+  </si>
+  <si>
+    <t>Salesman name</t>
+  </si>
+  <si>
+    <t>Use: Lookup Employee info by Salesman Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +767,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,8 +833,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -247,17 +905,299 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,29 +1601,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A40DD5A-2EA0-453B-B205-8D25B7B6EF10}">
-  <dimension ref="D4:N11"/>
+  <dimension ref="B4:N62"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A45" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="L4">
         <v>1</v>
       </c>
       <c r="M4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D5" s="4" t="s">
         <v>31</v>
       </c>
@@ -715,7 +1663,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
@@ -725,14 +1673,14 @@
       <c r="F6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="7">
         <f>VLOOKUP(D6,L5:M11,2,FALSE)</f>
         <v>5</v>
       </c>
       <c r="H6" s="5">
         <v>5000</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="7">
         <f>VLOOKUP(D6,L$5:N$11,3,FALSE)</f>
         <v>100000</v>
       </c>
@@ -749,7 +1697,11 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="7" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="29"/>
       <c r="D7" s="5" t="s">
         <v>26</v>
       </c>
@@ -783,7 +1735,9 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="8" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
@@ -817,7 +1771,9 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="9" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="5" t="s">
         <v>28</v>
       </c>
@@ -851,7 +1807,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="10" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D10" s="5" t="s">
         <v>29</v>
       </c>
@@ -885,7 +1841,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D11" s="5" t="s">
         <v>30</v>
       </c>
@@ -919,175 +1875,1115 @@
         <v>100000</v>
       </c>
     </row>
+    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="E15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="7" t="str">
+        <f>VLOOKUP(D19,L$18:N$28,2,FALSE)</f>
+        <v>Finance</v>
+      </c>
+      <c r="G19" s="7">
+        <f>VLOOKUP(D19,L$18:N$28,3,FALSE)</f>
+        <v>72704</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N19" s="6">
+        <v>30681</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="6" t="str">
+        <f t="shared" ref="F20:F28" si="2">VLOOKUP(D20,L$18:N$28,2,FALSE)</f>
+        <v>Operations</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" ref="G20:G28" si="3">VLOOKUP(D20,L$18:N$28,3,FALSE)</f>
+        <v>44718</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" s="6">
+        <v>44718</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Sales</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="3"/>
+        <v>35210</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="6">
+        <v>35210</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Finance</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="3"/>
+        <v>30681</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" s="6">
+        <v>72704</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Operations</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="3"/>
+        <v>47487</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N23" s="6">
+        <v>47487</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Operations</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N24" s="6">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D25" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Sales</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="3"/>
+        <v>63671</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N25" s="6">
+        <v>63671</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Finance</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="3"/>
+        <v>38966</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N26" s="6">
+        <v>38966</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Operations</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="3"/>
+        <v>77052</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N27" s="6">
+        <v>77052</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D28" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Sales</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="3"/>
+        <v>86570</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="6">
+        <v>86570</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D30" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>2</v>
+      </c>
+      <c r="N31" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D32" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="L32" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="M32" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="N32" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D33" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="21" t="str">
+        <f>VLOOKUP(D33,L32:N36,2,FALSE)</f>
+        <v>Riya Shah</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="21" t="str">
+        <f>VLOOKUP(D33,L32:N36,3,FALSE)</f>
+        <v>Mumbai</v>
+      </c>
+      <c r="L33" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="M33" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="N33" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B34" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="23" t="str">
+        <f t="shared" ref="E34:E36" si="4">VLOOKUP(D34,L33:N37,2,FALSE)</f>
+        <v>Arjun Mehta</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" s="23" t="str">
+        <f t="shared" ref="G34:G36" si="5">VLOOKUP(D34,L33:N37,3,FALSE)</f>
+        <v>Pune</v>
+      </c>
+      <c r="L34" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="M34" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="N34" s="23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="23" t="str">
+        <f t="shared" si="4"/>
+        <v>Sneha Roy</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="G35" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v>Delhi</v>
+      </c>
+      <c r="L35" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="M35" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="N35" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D36" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="23" t="str">
+        <f t="shared" si="4"/>
+        <v>Kunal Das</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v>Bangalore</v>
+      </c>
+      <c r="L36" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="M36" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N36" s="23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D38" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>2</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D40" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="L40" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="M40" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="N40" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D41" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="21" t="str">
+        <f>VLOOKUP(D41,L40:N44,2,FALSE)</f>
+        <v>Physics</v>
+      </c>
+      <c r="G41" s="21" t="str">
+        <f>VLOOKUP(D41,L40:N44,3,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="L41" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="M41" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="N41" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B42" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="F42" s="28" t="str">
+        <f t="shared" ref="F42:F44" si="6">VLOOKUP(D42,L41:N45,2,FALSE)</f>
+        <v>Chemistry</v>
+      </c>
+      <c r="G42" s="28" t="str">
+        <f t="shared" ref="G42:G44" si="7">VLOOKUP(D42,L41:N45,3,FALSE)</f>
+        <v>B</v>
+      </c>
+      <c r="L42" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="M42" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="N42" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="F43" s="28" t="str">
+        <f t="shared" si="6"/>
+        <v>Math</v>
+      </c>
+      <c r="G43" s="28" t="str">
+        <f t="shared" si="7"/>
+        <v>A+</v>
+      </c>
+      <c r="L43" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="M43" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="N43" s="28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D44" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="28" t="str">
+        <f>VLOOKUP(D44,L43:N48,2,FALSE)</f>
+        <v>Biology</v>
+      </c>
+      <c r="G44" s="28" t="str">
+        <f>VLOOKUP(D44,L43:N48,3,FALSE)</f>
+        <v>B+</v>
+      </c>
+      <c r="L44" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="M44" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="N44" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D46" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>2</v>
+      </c>
+      <c r="N47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D48" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="L48" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="M48" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="N48" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D49" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E49" s="21" t="str">
+        <f>VLOOKUP(D49,L48:N52,2,FALSE)</f>
+        <v>Air India</v>
+      </c>
+      <c r="F49" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="G49" s="21" t="str">
+        <f>VLOOKUP(D49,L48:N52,3,FALSE)</f>
+        <v>Dubai</v>
+      </c>
+      <c r="L49" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="M49" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="N49" s="25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B50" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E50" s="25" t="str">
+        <f>VLOOKUP(D50,L49:N52,2,FALSE)</f>
+        <v>Emirates</v>
+      </c>
+      <c r="F50" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G50" s="25" t="str">
+        <f>VLOOKUP(D50,L49:N52,3,FALSE)</f>
+        <v>London</v>
+      </c>
+      <c r="L50" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="M50" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="N50" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="E51" s="25" t="str">
+        <f>VLOOKUP(D51,L50:N53,2,FALSE)</f>
+        <v>British Air</v>
+      </c>
+      <c r="F51" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="G51" s="25" t="str">
+        <f>VLOOKUP(D51,L50:N53,3,FALSE)</f>
+        <v>New York</v>
+      </c>
+      <c r="L51" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="M51" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="N51" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D52" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="E52" s="25" t="str">
+        <f>VLOOKUP(D52,L51:N54,2,FALSE)</f>
+        <v>Lufthansa</v>
+      </c>
+      <c r="F52" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="G52" s="25" t="str">
+        <f>VLOOKUP(D52,L51:N54,3,FALSE)</f>
+        <v>Frankfurt</v>
+      </c>
+      <c r="L52" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="M52" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="N52" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D54" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>2</v>
+      </c>
+      <c r="N55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D56" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="G56" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="L56" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="M56" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="N56" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D57" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E57" s="21" t="str">
+        <f>VLOOKUP(D57,L56:N60,2,FALSE)</f>
+        <v>Nikhil Joshi</v>
+      </c>
+      <c r="F57" s="21" t="str">
+        <f>VLOOKUP(E57,M56:O60,2,FALSE)</f>
+        <v>Sedan</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="L57" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="M57" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="N57" s="26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B58" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E58" s="26" t="str">
+        <f t="shared" ref="E58:E60" si="8">VLOOKUP(D58,L57:N61,2,FALSE)</f>
+        <v>Priya Malhotra</v>
+      </c>
+      <c r="F58" s="26" t="str">
+        <f t="shared" ref="F58:F60" si="9">VLOOKUP(E58,M57:O61,2,FALSE)</f>
+        <v>SUV</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="L58" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="M58" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="N58" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="E59" s="26" t="str">
+        <f t="shared" si="8"/>
+        <v>Ravi Kumar</v>
+      </c>
+      <c r="F59" s="26" t="str">
+        <f t="shared" si="9"/>
+        <v>Hatchback</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="L59" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="M59" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="N59" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D60" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E60" s="26" t="str">
+        <f t="shared" si="8"/>
+        <v>Sneha Iyer</v>
+      </c>
+      <c r="F60" s="26" t="str">
+        <f t="shared" si="9"/>
+        <v>Bike</v>
+      </c>
+      <c r="G60" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="L60" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="M60" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="N60" s="26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D62" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+    </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B7:C9"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="B50:C51"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="B58:C59"/>
+    <mergeCell ref="E15:I16"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="D30:G30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5659DC8-1BEE-455C-A6E1-82BE9AD8C81E}">
-  <dimension ref="D6:L17"/>
+  <dimension ref="C3:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:J10"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" customWidth="1"/>
+    <col min="10" max="11" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="G3" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+    </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="5" t="str">
-        <f>HLOOKUP(E6,$D$15:$J$17,2,FALSE)</f>
+      <c r="F7" s="7" t="str">
+        <f>HLOOKUP(F6,$E$15:$K$17,2,FALSE)</f>
         <v>automotive sq, near tp road , 400001</v>
       </c>
-      <c r="F7" s="5" t="str">
-        <f t="shared" ref="F7:J7" si="0">HLOOKUP(F6,$D$15:$J$17,2,FALSE)</f>
+      <c r="G7" s="5" t="str">
+        <f>HLOOKUP(G6,$E$15:$K$17,2,FALSE)</f>
         <v>offline</v>
       </c>
-      <c r="G7" s="5">
-        <f t="shared" si="0"/>
+      <c r="H7" s="5">
+        <f>HLOOKUP(H6,$E$15:$K$17,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="H7" s="5">
-        <f t="shared" si="0"/>
+      <c r="I7" s="5">
+        <f>HLOOKUP(I6,$E$15:$K$17,2,FALSE)</f>
         <v>5000</v>
       </c>
-      <c r="I7" s="5">
-        <f t="shared" si="0"/>
+      <c r="J7" s="5">
+        <f>HLOOKUP(J6,$E$15:$K$17,2,FALSE)</f>
         <v>100000</v>
       </c>
-      <c r="J7" s="5">
-        <f t="shared" si="0"/>
+      <c r="K7" s="5">
+        <f>HLOOKUP(K6,$E$15:$K$17,2,FALSE)</f>
         <v>700</v>
       </c>
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="5">
         <v>2</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>1000</v>
       </c>
-      <c r="I8" s="5">
+      <c r="J8" s="5">
         <v>10000</v>
       </c>
-      <c r="J8" s="5">
+      <c r="K8" s="5">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <v>6</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>7000</v>
       </c>
-      <c r="I9" s="5">
+      <c r="J9" s="5">
         <v>200000</v>
       </c>
-      <c r="J9" s="5">
+      <c r="K9" s="5">
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="5" t="str">
-        <f>HLOOKUP(E6,$D$15:$J$17,3,FALSE)</f>
+      <c r="F10" s="7" t="str">
+        <f>HLOOKUP(F6,$E$15:$K$17,3,FALSE)</f>
         <v>nandanvan</v>
       </c>
-      <c r="F10" s="5" t="str">
-        <f t="shared" ref="F10:J10" si="1">HLOOKUP(F6,$D$15:$J$17,3,FALSE)</f>
+      <c r="G10" s="5" t="str">
+        <f>HLOOKUP(G6,$E$15:$K$17,3,FALSE)</f>
         <v>online</v>
       </c>
-      <c r="G10" s="5">
-        <f t="shared" si="1"/>
+      <c r="H10" s="5">
+        <f>HLOOKUP(H6,$E$15:$K$17,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="H10" s="5">
-        <f t="shared" si="1"/>
+      <c r="I10" s="5">
+        <f>HLOOKUP(I6,$E$15:$K$17,3,FALSE)</f>
         <v>15000</v>
       </c>
-      <c r="I10" s="5">
-        <f t="shared" si="1"/>
+      <c r="J10" s="5">
+        <f>HLOOKUP(J6,$E$15:$K$17,3,FALSE)</f>
         <v>200000</v>
       </c>
-      <c r="J10" s="5">
-        <f t="shared" si="1"/>
+      <c r="K10" s="5">
+        <f>HLOOKUP(K6,$E$15:$K$17,3,FALSE)</f>
         <v>5000</v>
       </c>
     </row>
     <row r="11" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="5">
+      <c r="H11" s="5">
         <v>3</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <v>12000</v>
       </c>
-      <c r="I11" s="5">
+      <c r="J11" s="5">
         <v>150000</v>
       </c>
-      <c r="J11" s="5">
+      <c r="K11" s="5">
         <v>7000</v>
       </c>
       <c r="L11" t="s">
@@ -1095,98 +2991,1067 @@
       </c>
     </row>
     <row r="12" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="5">
+      <c r="H12" s="5">
         <v>10</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>2000</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>50000</v>
       </c>
-      <c r="J12" s="5">
+      <c r="K12" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D15" s="4" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D16" s="5" t="s">
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="5">
+      <c r="G16" s="5">
         <v>700</v>
       </c>
-      <c r="G16" s="5">
+      <c r="H16" s="5">
         <v>5</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="5">
         <v>100000</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="5">
+      <c r="K16" s="5">
         <v>5000</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D17" s="5" t="s">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="5">
+      <c r="G17" s="5">
         <v>5000</v>
       </c>
-      <c r="G17" s="5">
+      <c r="H17" s="5">
         <v>1</v>
       </c>
-      <c r="H17" s="5">
+      <c r="I17" s="5">
         <v>200000</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="5">
+      <c r="K17" s="5">
         <v>15000</v>
       </c>
     </row>
+    <row r="20" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
+    </row>
+    <row r="22" spans="3:11" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="20"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="7" t="str">
+        <f>HLOOKUP(F24,E36:J38,2,FALSE)</f>
+        <v>Employee_1</v>
+      </c>
+      <c r="G25" s="6" t="str">
+        <f>HLOOKUP(G24,F36:K38,2,FALSE)</f>
+        <v>Finance</v>
+      </c>
+      <c r="H25" s="6">
+        <f>HLOOKUP(H24,G36:L38,2,FALSE)</f>
+        <v>72704</v>
+      </c>
+      <c r="I25" s="6" t="str">
+        <f>HLOOKUP(I24,H36:M38,2,FALSE)</f>
+        <v>completed</v>
+      </c>
+      <c r="J25" s="6">
+        <f>HLOOKUP(J24,I36:N38,2,FALSE)</f>
+        <v>10905.6</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E26" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="6">
+        <v>44718</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J26" s="6">
+        <v>4471.8</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="6">
+        <v>35210</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J27" s="6">
+        <v>3521</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="6">
+        <v>30681</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J28" s="6">
+        <v>3068.1000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" s="6" t="str">
+        <f>HLOOKUP(F24,C36:H38,3,FALSE)</f>
+        <v>Employee_5</v>
+      </c>
+      <c r="G29" s="6" t="str">
+        <f>HLOOKUP(G24,D36:I38,3,FALSE)</f>
+        <v>Operations</v>
+      </c>
+      <c r="H29" s="7">
+        <f>HLOOKUP(H24,E36:J38,3,FALSE)</f>
+        <v>47487</v>
+      </c>
+      <c r="I29" s="6" t="str">
+        <f>HLOOKUP(I24,F36:K38,3,FALSE)</f>
+        <v>incomplete</v>
+      </c>
+      <c r="J29" s="6">
+        <f>HLOOKUP(J24,G36:L38,3,FALSE)</f>
+        <v>4748.7</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="6">
+        <v>30000</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" s="6">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E31" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" s="6">
+        <v>63671</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J31" s="6">
+        <v>9550.65</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="E32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="6">
+        <v>38966</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J32" s="6">
+        <v>3896.6000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E33" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" s="6">
+        <v>77052</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J33" s="6">
+        <v>15410.400000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E34" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H34" s="6">
+        <v>86570</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J34" s="6">
+        <v>17314</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37" s="6">
+        <v>72704</v>
+      </c>
+      <c r="I37" s="6">
+        <v>10905.6</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H38" s="6">
+        <v>47487</v>
+      </c>
+      <c r="I38" s="6">
+        <v>4748.7</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E40" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E42" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="I42" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="J42" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C43" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" s="14"/>
+      <c r="E43" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="F43" s="21">
+        <f>HLOOKUP(F42,$E47:$J49,2,FALSE)</f>
+        <v>15000</v>
+      </c>
+      <c r="G43" s="31">
+        <f t="shared" ref="G43:J43" si="0">HLOOKUP(G42,$E47:$J49,2,FALSE)</f>
+        <v>20000</v>
+      </c>
+      <c r="H43" s="31">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="I43" s="31">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+      <c r="J43" s="31">
+        <f>HLOOKUP(J42,$E47:$J49,2,FALSE)</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="F44" s="31">
+        <f>HLOOKUP(F43,E48:J50,2,FALSE)</f>
+        <v>2000</v>
+      </c>
+      <c r="G44" s="31">
+        <v>5200</v>
+      </c>
+      <c r="H44" s="31">
+        <v>5100</v>
+      </c>
+      <c r="I44" s="31">
+        <v>5300</v>
+      </c>
+      <c r="J44" s="31">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E45" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="F45" s="21">
+        <f>HLOOKUP(F42,$E47:$J49,3,FALSE)</f>
+        <v>2000</v>
+      </c>
+      <c r="G45" s="31">
+        <f t="shared" ref="G45:J45" si="1">HLOOKUP(G42,$E47:$J49,3,FALSE)</f>
+        <v>1800</v>
+      </c>
+      <c r="H45" s="31">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="I45" s="31">
+        <f>HLOOKUP(I42,$E47:$J49,3,FALSE)</f>
+        <v>2100</v>
+      </c>
+      <c r="J45" s="31">
+        <f t="shared" si="1"/>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G47" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="H47" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="I47" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="J47" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="F48" s="31">
+        <v>15000</v>
+      </c>
+      <c r="G48" s="31">
+        <v>20000</v>
+      </c>
+      <c r="H48" s="31">
+        <v>1500</v>
+      </c>
+      <c r="I48" s="31">
+        <v>15000</v>
+      </c>
+      <c r="J48" s="31">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="F49" s="31">
+        <v>2000</v>
+      </c>
+      <c r="G49" s="31">
+        <v>1800</v>
+      </c>
+      <c r="H49" s="31">
+        <v>2200</v>
+      </c>
+      <c r="I49" s="31">
+        <v>2100</v>
+      </c>
+      <c r="J49" s="31">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E51" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E53" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="G53" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="H53" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="I53" s="30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C54" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="F54" s="21">
+        <f>HLOOKUP(F53,$E58:$I60,2,FALSE)</f>
+        <v>25000</v>
+      </c>
+      <c r="G54" s="33">
+        <f t="shared" ref="G54:I54" si="2">HLOOKUP(G53,$E58:$I60,2,FALSE)</f>
+        <v>27000</v>
+      </c>
+      <c r="H54" s="33">
+        <f t="shared" si="2"/>
+        <v>23000</v>
+      </c>
+      <c r="I54" s="33">
+        <f>HLOOKUP(I53,$E58:$I60,2,FALSE)</f>
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="F55" s="33">
+        <v>10</v>
+      </c>
+      <c r="G55" s="33">
+        <v>12</v>
+      </c>
+      <c r="H55" s="33">
+        <v>8</v>
+      </c>
+      <c r="I55" s="33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E56" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="F56" s="21">
+        <f>HLOOKUP(F53,$E58:$I60,3,FALSE)</f>
+        <v>1.2</v>
+      </c>
+      <c r="G56" s="33">
+        <f t="shared" ref="G56:I56" si="3">HLOOKUP(G53,$E58:$I60,3,FALSE)</f>
+        <v>1.3</v>
+      </c>
+      <c r="H56" s="33">
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I56" s="33">
+        <f>HLOOKUP(I53,$E58:$I60,3,FALSE)</f>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E58" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="F58" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="G58" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="H58" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="I58" s="30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E59" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="F59" s="33">
+        <v>25000</v>
+      </c>
+      <c r="G59" s="33">
+        <v>27000</v>
+      </c>
+      <c r="H59" s="33">
+        <v>23000</v>
+      </c>
+      <c r="I59" s="33">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E60" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="F60" s="33">
+        <v>1.2</v>
+      </c>
+      <c r="G60" s="33">
+        <v>1.3</v>
+      </c>
+      <c r="H60" s="33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I60" s="33">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E62" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="F62" s="32"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="I62" s="32"/>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E64" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F64" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="G64" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="H64" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="I64" s="30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C65" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D65" s="14"/>
+      <c r="E65" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F65" s="21">
+        <f>HLOOKUP(F64,$E69:$I71,2,FALSE)</f>
+        <v>88</v>
+      </c>
+      <c r="G65" s="26">
+        <f t="shared" ref="G65:I65" si="4">HLOOKUP(G64,$E69:$I71,2,FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="H65" s="26">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="I65" s="26">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="F66" s="26">
+        <f>HLOOKUP(F64,$E69:$I71,3,FALSE)</f>
+        <v>92</v>
+      </c>
+      <c r="G66" s="26">
+        <f t="shared" ref="G66:I66" si="5">HLOOKUP(G64,$E69:$I71,3,FALSE)</f>
+        <v>81</v>
+      </c>
+      <c r="H66" s="26">
+        <f t="shared" si="5"/>
+        <v>89</v>
+      </c>
+      <c r="I66" s="26">
+        <f>HLOOKUP(I64,$E69:$I71,3,FALSE)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E67" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="F67" s="21">
+        <v>85</v>
+      </c>
+      <c r="G67" s="26">
+        <v>79</v>
+      </c>
+      <c r="H67" s="26">
+        <v>94</v>
+      </c>
+      <c r="I67" s="26">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E69" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F69" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="G69" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="H69" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="I69" s="30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E70" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F70" s="26">
+        <v>88</v>
+      </c>
+      <c r="G70" s="26">
+        <v>76</v>
+      </c>
+      <c r="H70" s="26">
+        <v>90</v>
+      </c>
+      <c r="I70" s="26">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E71" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="F71" s="26">
+        <v>92</v>
+      </c>
+      <c r="G71" s="26">
+        <v>81</v>
+      </c>
+      <c r="H71" s="26">
+        <v>89</v>
+      </c>
+      <c r="I71" s="26">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E73" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="F73" s="35"/>
+      <c r="G73" s="35"/>
+      <c r="H73" s="35"/>
+      <c r="I73" s="36"/>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E75" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F75" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G75" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="H75" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="I75" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="J75" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E76" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="F76" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="G76" s="37"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="37"/>
+      <c r="J76" s="37"/>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C77" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D77" s="14"/>
+      <c r="E77" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="F77" s="21">
+        <f>HLOOKUP(F75,$E81:$J83,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G77" s="37">
+        <f t="shared" ref="G77:J77" si="6">HLOOKUP(G75,$E81:$J83,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H77" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v>✔</v>
+      </c>
+      <c r="I77" s="37">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J77" s="37">
+        <f>HLOOKUP(J75,$E81:$J83,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="F78" s="37"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="J78" s="37"/>
+    </row>
+    <row r="79" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E79" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="F79" s="21">
+        <f>HLOOKUP(F75,$E81:$J83,3,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G79" s="37">
+        <f t="shared" ref="G79:J79" si="7">HLOOKUP(G75,$E81:$J83,3,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H79" s="37">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I79" s="37">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J79" s="37" t="str">
+        <f>HLOOKUP(J75,$E81:$J83,3,FALSE)</f>
+        <v>✔</v>
+      </c>
+    </row>
+    <row r="81" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E81" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="F81" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G81" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="H81" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="I81" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="J81" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E82" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="I82" s="37"/>
+      <c r="J82" s="37"/>
+    </row>
+    <row r="83" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E83" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="F83" s="37"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+      <c r="J83" s="37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="85" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E85" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="F85" s="32"/>
+      <c r="G85" s="32"/>
+      <c r="H85" s="32"/>
+      <c r="I85" s="32"/>
+      <c r="J85" s="32"/>
+    </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="E85:J85"/>
+    <mergeCell ref="C77:D78"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E62:I62"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="C65:D66"/>
+    <mergeCell ref="E73:I73"/>
+    <mergeCell ref="E21:I22"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="G3:I5"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="C43:D44"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>